<commit_message>
updated excel with precision and recall of models
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Desktop\DesEng\Data science\Group project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2000F862-0F0F-43B0-B0B9-887A55E0BA43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04767875-8C08-47E0-90D7-7B6AEC614307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="83" yWindow="98" windowWidth="11947" windowHeight="15479" xr2:uid="{16500657-6E1E-4564-929F-E4AA0CA5EF83}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Variables in model</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>PTEBACHUM_E_PTQ_EE, P8MEA_17, PTEBACLAN_E_PTQ_EE</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>VALIDATION</t>
+  </si>
+  <si>
+    <t>Recall</t>
   </si>
 </sst>
 </file>
@@ -98,9 +110,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,66 +433,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B76A8A-A239-4DF5-B503-7DD170EC146A}">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="59.46484375" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.97099999999999997</v>
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="F3">
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.97099999999999997</v>
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="F4">
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.97099999999999997</v>
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="F5">
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.97099999999999997</v>
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="F6">
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.88200000000000001</v>
+        <v>0.79411764705882304</v>
+      </c>
+      <c r="D7">
+        <v>0.75</v>
+      </c>
+      <c r="E7">
+        <v>0.8</v>
+      </c>
+      <c r="F7">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="G7">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="H7">
+        <v>0.88235294117647001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added meta data to models so easier to understand
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Desktop\DesEng\Data science\Group project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04767875-8C08-47E0-90D7-7B6AEC614307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D5BE6-664C-4855-B342-BE343ACD9393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="83" yWindow="98" windowWidth="11947" windowHeight="15479" xr2:uid="{16500657-6E1E-4564-929F-E4AA0CA5EF83}"/>
+    <workbookView xWindow="12263" yWindow="210" windowWidth="11947" windowHeight="15480" xr2:uid="{16500657-6E1E-4564-929F-E4AA0CA5EF83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Variables in model</t>
   </si>
@@ -67,13 +67,52 @@
   </si>
   <si>
     <t>Recall</t>
+  </si>
+  <si>
+    <t>Meta data</t>
+  </si>
+  <si>
+    <t>P8MEA</t>
+  </si>
+  <si>
+    <t>KS2APS</t>
+  </si>
+  <si>
+    <t>P8MEA_17</t>
+  </si>
+  <si>
+    <t>ATT8SCR_17</t>
+  </si>
+  <si>
+    <t>PTEBACHUM_E_PTQ_EE</t>
+  </si>
+  <si>
+    <t>TEBACLAN_E_PTQ_EE</t>
+  </si>
+  <si>
+    <t>Progress 8 measure after adjustment for extreme scores (2019)</t>
+  </si>
+  <si>
+    <t>Key stage 2 Average Points Score of the cohort at the end of key stage 4</t>
+  </si>
+  <si>
+    <t>Progress 8 measure after adjustment for extreme scores (2017)</t>
+  </si>
+  <si>
+    <t>Attainment 8 score (2017)</t>
+  </si>
+  <si>
+    <t>% of pupils entering the English Baccalaureate Humanities subject area</t>
+  </si>
+  <si>
+    <t>% of pupils entering the English Baccalaureate Language subject area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +124,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,10 +158,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -433,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B76A8A-A239-4DF5-B503-7DD170EC146A}">
-  <dimension ref="B1:H7"/>
+  <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -451,16 +496,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
@@ -598,6 +643,59 @@
       </c>
       <c r="H7">
         <v>0.88235294117647001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -605,6 +703,7 @@
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
removed P8MEA from forward selection, found new models and evaluated them
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Desktop\DesEng\Data science\Group project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D5BE6-664C-4855-B342-BE343ACD9393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451CB81D-80F1-4E2C-890F-2388A841DE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12263" yWindow="210" windowWidth="11947" windowHeight="15480" xr2:uid="{16500657-6E1E-4564-929F-E4AA0CA5EF83}"/>
+    <workbookView xWindow="98" yWindow="23" windowWidth="11947" windowHeight="15480" xr2:uid="{16500657-6E1E-4564-929F-E4AA0CA5EF83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Variables in model</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>% of pupils entering the English Baccalaureate Language subject area</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>P8MEA_17, KS2APS, PTFSM6CLA1A</t>
+  </si>
+  <si>
+    <t>ATT8SCR_17, TOTPUPS, PTEBACMAT_E_PTQ_EE</t>
+  </si>
+  <si>
+    <t>KS2APS, TOTPUPS</t>
   </si>
 </sst>
 </file>
@@ -135,12 +150,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -164,6 +185,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,14 +501,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B76A8A-A239-4DF5-B503-7DD170EC146A}">
-  <dimension ref="B1:H15"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="9.06640625" style="1"/>
     <col min="2" max="2" width="59.46484375" customWidth="1"/>
     <col min="3" max="3" width="13.86328125" customWidth="1"/>
     <col min="4" max="4" width="13.1328125" customWidth="1"/>
@@ -495,67 +519,49 @@
     <col min="8" max="8" width="13.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B2" s="1" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>2</v>
-      </c>
-      <c r="C3">
-        <v>0.97058823529411697</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.93333333333333302</v>
-      </c>
-      <c r="F3">
-        <v>0.97058823529411697</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0.94117647058823495</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>3</v>
       </c>
       <c r="C4">
         <v>0.97058823529411697</v>
@@ -576,9 +582,9 @@
         <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0.97058823529411697</v>
@@ -599,9 +605,9 @@
         <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>0.97058823529411697</v>
@@ -622,86 +628,171 @@
         <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="F7">
+        <v>0.97058823529411697</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.94117647058823495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>0.79411764705882304</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>0.75</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>0.8</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>0.88235294117647001</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>0.88235294117647001</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>0.88235294117647001</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
+  <mergeCells count="4">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added values for accuracy, recall and precision for new models to excel sheet
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Desktop\DesEng\Data science\Group project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451CB81D-80F1-4E2C-890F-2388A841DE47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D1BB0-785E-4403-AFD4-434BA4402661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="98" yWindow="23" windowWidth="11947" windowHeight="15480" xr2:uid="{16500657-6E1E-4564-929F-E4AA0CA5EF83}"/>
   </bookViews>
@@ -179,14 +179,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B76A8A-A239-4DF5-B503-7DD170EC146A}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -519,22 +519,22 @@
     <col min="8" max="8" width="13.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
@@ -727,22 +727,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
@@ -771,20 +771,92 @@
       <c r="B21" t="s">
         <v>26</v>
       </c>
+      <c r="C21">
+        <v>0.91176470588235203</v>
+      </c>
+      <c r="D21">
+        <v>0.875</v>
+      </c>
+      <c r="E21">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="F21">
+        <v>0.91176470588235203</v>
+      </c>
+      <c r="G21">
+        <v>0.9375</v>
+      </c>
+      <c r="H21">
+        <v>0.88235294117647001</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>27</v>
       </c>
+      <c r="C22">
+        <v>0.91176470588235203</v>
+      </c>
+      <c r="D22">
+        <v>0.875</v>
+      </c>
+      <c r="E22">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="F22">
+        <v>0.91176470588235203</v>
+      </c>
+      <c r="G22">
+        <v>0.9375</v>
+      </c>
+      <c r="H22">
+        <v>0.88235294117647001</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>28</v>
       </c>
+      <c r="C23">
+        <v>0.82352941176470495</v>
+      </c>
+      <c r="D23">
+        <v>0.76470588235294101</v>
+      </c>
+      <c r="E23">
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="F23">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="G23">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="H23">
+        <v>0.82352941176470495</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>6</v>
+      </c>
+      <c r="C24">
+        <v>0.79411764705882304</v>
+      </c>
+      <c r="D24">
+        <v>0.75</v>
+      </c>
+      <c r="E24">
+        <v>0.8</v>
+      </c>
+      <c r="F24">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="G24">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="H24">
+        <v>0.88235294117647001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>